<commit_message>
Adding new reports; Power BI enhacement
Adição de novos relatórios de corrida e aperfeiçoamento da exibição visual do Power BI.
</commit_message>
<xml_diff>
--- a/corridas.xlsx
+++ b/corridas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ed13a9f75b3f891/Documentos/EstudosRPA/RUNNING_RPA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_5FAD55D891706E0E62355476585DCE3A87477B1B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D72B00A-F140-47B8-939B-075808127322}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2BA594109559FE0E62355476585DCE3A87479168" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B506546-5A10-46DB-8046-2DD93794B3E1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="269">
   <si>
     <t>arquivo</t>
   </si>
@@ -698,15 +698,141 @@
   </si>
   <si>
     <t>00:29:08</t>
+  </si>
+  <si>
+    <t>recorte_1751669290178.jpg</t>
+  </si>
+  <si>
+    <t>2025-05-14 20:04</t>
+  </si>
+  <si>
+    <t>05'50"</t>
+  </si>
+  <si>
+    <t>00:29:27</t>
+  </si>
+  <si>
+    <t>recorte_1751669307802.jpg</t>
+  </si>
+  <si>
+    <t>2025-05-21 19:54</t>
+  </si>
+  <si>
+    <t>08'05"</t>
+  </si>
+  <si>
+    <t>00:24:39</t>
+  </si>
+  <si>
+    <t>recorte_1751669319061.jpg</t>
+  </si>
+  <si>
+    <t>recorte_1751669329739.jpg</t>
+  </si>
+  <si>
+    <t>2025-05-22 20:58</t>
+  </si>
+  <si>
+    <t>00:32:07</t>
+  </si>
+  <si>
+    <t>recorte_1751669342043.jpg</t>
+  </si>
+  <si>
+    <t>2025-05-24 08:19</t>
+  </si>
+  <si>
+    <t>06'02"</t>
+  </si>
+  <si>
+    <t>00:30:12</t>
+  </si>
+  <si>
+    <t>recorte_1751669353512.jpg</t>
+  </si>
+  <si>
+    <t>2025-05-30 18:52</t>
+  </si>
+  <si>
+    <t>07'19"</t>
+  </si>
+  <si>
+    <t>00:21:58</t>
+  </si>
+  <si>
+    <t>recorte_1751669364774.jpg</t>
+  </si>
+  <si>
+    <t>2025-06-01 08:02</t>
+  </si>
+  <si>
+    <t>05'41"</t>
+  </si>
+  <si>
+    <t>00:30:03</t>
+  </si>
+  <si>
+    <t>recorte_1751669373188.jpg</t>
+  </si>
+  <si>
+    <t>2025-06-18 20:29</t>
+  </si>
+  <si>
+    <t>06'47"</t>
+  </si>
+  <si>
+    <t>00:33:56</t>
+  </si>
+  <si>
+    <t>recorte_1751669381275.jpg</t>
+  </si>
+  <si>
+    <t>2025-06-29 17:52</t>
+  </si>
+  <si>
+    <t>06'45"</t>
+  </si>
+  <si>
+    <t>00:33:47</t>
+  </si>
+  <si>
+    <t>recorte_1751669398173.jpg</t>
+  </si>
+  <si>
+    <t>2025-07-04 17:23</t>
+  </si>
+  <si>
+    <t>05'56"</t>
+  </si>
+  <si>
+    <t>00:25:13</t>
+  </si>
+  <si>
+    <t>recorte_1751669409341.jpg</t>
+  </si>
+  <si>
+    <t>2025-07-04 19:00</t>
+  </si>
+  <si>
+    <t>00:26:35</t>
+  </si>
+  <si>
+    <t>recorte_1752158007844.jpg</t>
+  </si>
+  <si>
+    <t>2025-07-09 10:26</t>
+  </si>
+  <si>
+    <t>06'48"</t>
+  </si>
+  <si>
+    <t>01:08:07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -756,12 +882,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1064,23 +1189,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J58"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1117,700 +1242,700 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
       <c r="D2">
-        <v>2.5099999999999998</v>
+        <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G2">
-        <v>267</v>
+        <v>426</v>
       </c>
       <c r="H2">
-        <v>1890</v>
+        <v>3889</v>
       </c>
       <c r="I2">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="J2">
-        <v>132</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3">
-        <v>3.21</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="E3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G3">
-        <v>342</v>
+        <v>428</v>
       </c>
       <c r="H3">
-        <v>1436</v>
+        <v>3675</v>
       </c>
       <c r="I3">
-        <v>47</v>
+        <v>137</v>
       </c>
       <c r="J3">
-        <v>223</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="D4">
-        <v>3.08</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G4">
-        <v>328</v>
+        <v>267</v>
       </c>
       <c r="H4">
-        <v>372</v>
+        <v>1890</v>
       </c>
       <c r="I4">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="J4">
-        <v>828</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
       </c>
       <c r="D5">
-        <v>3.42</v>
+        <v>3.21</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G5">
-        <v>365</v>
+        <v>342</v>
       </c>
       <c r="H5">
-        <v>2031</v>
+        <v>1436</v>
       </c>
       <c r="I5">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="J5">
-        <v>168</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
       <c r="D6">
-        <v>8.1</v>
+        <v>3.08</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="G6">
-        <v>863</v>
+        <v>328</v>
       </c>
       <c r="H6">
-        <v>5597</v>
+        <v>372</v>
       </c>
       <c r="I6">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="J6">
-        <v>144</v>
+        <v>828</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
       </c>
       <c r="D7">
-        <v>6.76</v>
+        <v>3.42</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="G7">
-        <v>720</v>
+        <v>365</v>
       </c>
       <c r="H7">
-        <v>3643</v>
+        <v>2031</v>
       </c>
       <c r="I7">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="J7">
-        <v>185</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
       <c r="D8">
-        <v>5.04</v>
+        <v>8.1</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="G8">
-        <v>538</v>
+        <v>863</v>
       </c>
       <c r="H8">
-        <v>2178</v>
+        <v>5597</v>
       </c>
       <c r="I8">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="J8">
-        <v>231</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
       </c>
       <c r="D9">
-        <v>3.33</v>
+        <v>6.76</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G9">
-        <v>355</v>
+        <v>720</v>
       </c>
       <c r="H9">
-        <v>1578</v>
+        <v>3643</v>
       </c>
       <c r="I9">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J9">
-        <v>211</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>43</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
       <c r="D10">
-        <v>4.0199999999999996</v>
+        <v>5.04</v>
       </c>
       <c r="E10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="G10">
-        <v>429</v>
+        <v>538</v>
       </c>
       <c r="H10">
-        <v>1809</v>
+        <v>2178</v>
       </c>
       <c r="I10">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J10">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>3.33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11">
+        <v>355</v>
+      </c>
+      <c r="H11">
+        <v>1578</v>
+      </c>
+      <c r="I11">
         <v>55</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>3.01</v>
-      </c>
-      <c r="E11" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11">
-        <v>320</v>
-      </c>
-      <c r="H11">
-        <v>1409</v>
-      </c>
-      <c r="I11">
-        <v>67</v>
-      </c>
       <c r="J11">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
       </c>
       <c r="D12">
-        <v>3.08</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="E12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="G12">
-        <v>328</v>
+        <v>429</v>
       </c>
       <c r="H12">
-        <v>1170</v>
+        <v>1809</v>
       </c>
       <c r="I12">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="J12">
-        <v>263</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="D13">
-        <v>2.96</v>
+        <v>3.01</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="G13">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="H13">
-        <v>1160</v>
+        <v>1409</v>
       </c>
       <c r="I13">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="J13">
-        <v>255</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>3.08</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G14">
-        <v>320</v>
+        <v>328</v>
       </c>
       <c r="H14">
-        <v>2453</v>
+        <v>1170</v>
       </c>
       <c r="I14">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="J14">
-        <v>122</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>72</v>
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>2.96</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F15" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G15">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="H15">
-        <v>1250</v>
+        <v>1160</v>
       </c>
       <c r="I15">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="J15">
-        <v>239</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
+      </c>
+      <c r="B16" t="s">
+        <v>68</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16">
-        <v>2.67</v>
+        <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="G16">
-        <v>284</v>
+        <v>320</v>
       </c>
       <c r="H16">
-        <v>1506</v>
+        <v>2453</v>
       </c>
       <c r="I16">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="J16">
-        <v>177</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
+        <v>72</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="G17">
-        <v>373</v>
+        <v>320</v>
       </c>
       <c r="H17">
-        <v>1619</v>
+        <v>1250</v>
       </c>
       <c r="I17">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J17">
-        <v>216</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>84</v>
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18">
-        <v>3.51</v>
+        <v>2.67</v>
       </c>
       <c r="E18" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="G18">
-        <v>374</v>
+        <v>284</v>
       </c>
       <c r="H18">
-        <v>2709</v>
+        <v>1506</v>
       </c>
       <c r="I18">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="J18">
-        <v>129</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>88</v>
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19">
-        <v>3.06</v>
+        <v>3.5</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G19">
-        <v>325</v>
+        <v>373</v>
       </c>
       <c r="H19">
-        <v>2897</v>
+        <v>1619</v>
       </c>
       <c r="I19">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="J19">
-        <v>105</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
+      </c>
+      <c r="B20" t="s">
+        <v>84</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20">
-        <v>3.06</v>
+        <v>3.51</v>
       </c>
       <c r="E20" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="F20" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G20">
-        <v>326</v>
+        <v>374</v>
       </c>
       <c r="H20">
-        <v>2786</v>
+        <v>2709</v>
       </c>
       <c r="I20">
+        <v>108</v>
+      </c>
+      <c r="J20">
         <v>129</v>
-      </c>
-      <c r="J20">
-        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
+      </c>
+      <c r="B21" t="s">
+        <v>88</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
       </c>
       <c r="D21">
-        <v>5.55</v>
+        <v>3.06</v>
       </c>
       <c r="E21" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F21" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G21">
-        <v>592</v>
+        <v>325</v>
       </c>
       <c r="H21">
-        <v>5173</v>
+        <v>2897</v>
       </c>
       <c r="I21">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="J21">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
       <c r="D22">
-        <v>3.56</v>
+        <v>3.06</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F22" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G22">
-        <v>379</v>
+        <v>326</v>
       </c>
       <c r="H22">
-        <v>3394</v>
+        <v>2786</v>
       </c>
       <c r="I22">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="J22">
-        <v>104</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
       </c>
       <c r="D23">
-        <v>3.2</v>
+        <v>5.55</v>
       </c>
       <c r="E23" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F23" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G23">
-        <v>341</v>
+        <v>592</v>
       </c>
       <c r="H23">
-        <v>2972</v>
+        <v>5173</v>
       </c>
       <c r="I23">
         <v>128</v>
@@ -1821,713 +1946,713 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>107</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
+      </c>
+      <c r="B24" t="s">
+        <v>100</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
       </c>
       <c r="D24">
-        <v>3.04</v>
+        <v>3.56</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F24" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G24">
-        <v>324</v>
+        <v>379</v>
       </c>
       <c r="H24">
-        <v>2736</v>
+        <v>3394</v>
       </c>
       <c r="I24">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="J24">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>111</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
       </c>
       <c r="D25">
-        <v>1.5</v>
+        <v>3.2</v>
       </c>
       <c r="E25" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="F25" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="G25">
-        <v>160</v>
+        <v>341</v>
       </c>
       <c r="H25">
-        <v>1319</v>
+        <v>2972</v>
       </c>
       <c r="I25">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="J25">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>115</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
       <c r="D26">
-        <v>4.05</v>
+        <v>3.04</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="F26" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G26">
-        <v>431</v>
+        <v>324</v>
       </c>
       <c r="H26">
-        <v>3918</v>
+        <v>2736</v>
       </c>
       <c r="I26">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J26">
-        <v>103</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>118</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
+      </c>
+      <c r="B27" t="s">
+        <v>112</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
       </c>
       <c r="D27">
-        <v>3.02</v>
+        <v>1.5</v>
       </c>
       <c r="E27" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F27" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G27">
-        <v>322</v>
+        <v>160</v>
       </c>
       <c r="H27">
-        <v>2709</v>
+        <v>1319</v>
       </c>
       <c r="I27">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="J27">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>122</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
+      </c>
+      <c r="B28" t="s">
+        <v>116</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
       </c>
       <c r="D28">
-        <v>4.1399999999999997</v>
+        <v>4.05</v>
       </c>
       <c r="E28" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="F28" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G28">
-        <v>441</v>
+        <v>431</v>
       </c>
       <c r="H28">
-        <v>4262</v>
+        <v>3918</v>
       </c>
       <c r="I28">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="J28">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>127</v>
+        <v>118</v>
+      </c>
+      <c r="B29" t="s">
+        <v>119</v>
       </c>
       <c r="C29" t="s">
         <v>12</v>
       </c>
       <c r="D29">
-        <v>5.29</v>
+        <v>3.02</v>
       </c>
       <c r="E29" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="F29" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G29">
-        <v>564</v>
+        <v>322</v>
       </c>
       <c r="H29">
-        <v>5379</v>
+        <v>2709</v>
       </c>
       <c r="I29">
         <v>136</v>
       </c>
       <c r="J29">
-        <v>98</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>129</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
+      </c>
+      <c r="B30" t="s">
+        <v>123</v>
       </c>
       <c r="C30" t="s">
         <v>12</v>
       </c>
       <c r="D30">
-        <v>4.4000000000000004</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="F30" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="G30">
-        <v>468</v>
+        <v>441</v>
       </c>
       <c r="H30">
-        <v>4280</v>
+        <v>4262</v>
       </c>
       <c r="I30">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="J30">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>132</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
+      </c>
+      <c r="B31" t="s">
+        <v>127</v>
       </c>
       <c r="C31" t="s">
         <v>12</v>
       </c>
       <c r="D31">
-        <v>5.0599999999999996</v>
+        <v>5.29</v>
       </c>
       <c r="E31" t="s">
-        <v>134</v>
+        <v>69</v>
       </c>
       <c r="F31" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="G31">
-        <v>540</v>
+        <v>564</v>
       </c>
       <c r="H31">
-        <v>5195</v>
+        <v>5379</v>
       </c>
       <c r="I31">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="J31">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>136</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
+      </c>
+      <c r="B32" t="s">
+        <v>130</v>
       </c>
       <c r="C32" t="s">
         <v>12</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E32" t="s">
-        <v>138</v>
+        <v>73</v>
       </c>
       <c r="F32" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="G32">
-        <v>426</v>
+        <v>468</v>
       </c>
       <c r="H32">
-        <v>4145</v>
+        <v>4280</v>
       </c>
       <c r="I32">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J32">
-        <v>96</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>140</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>141</v>
+        <v>132</v>
+      </c>
+      <c r="B33" t="s">
+        <v>133</v>
       </c>
       <c r="C33" t="s">
         <v>12</v>
       </c>
       <c r="D33">
-        <v>5.0199999999999996</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>134</v>
       </c>
       <c r="F33" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G33">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="H33">
-        <v>5095</v>
+        <v>5195</v>
       </c>
       <c r="I33">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="J33">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>143</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
+      </c>
+      <c r="B34" t="s">
+        <v>137</v>
       </c>
       <c r="C34" t="s">
         <v>12</v>
       </c>
       <c r="D34">
-        <v>6.02</v>
+        <v>4</v>
       </c>
       <c r="E34" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F34" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="G34">
-        <v>642</v>
+        <v>426</v>
       </c>
       <c r="H34">
-        <v>7196</v>
+        <v>4145</v>
       </c>
       <c r="I34">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="J34">
-        <v>83</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>147</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
+      </c>
+      <c r="B35" t="s">
+        <v>141</v>
       </c>
       <c r="C35" t="s">
         <v>12</v>
       </c>
       <c r="D35">
-        <v>3.8</v>
+        <v>5.0199999999999996</v>
       </c>
       <c r="E35" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
       <c r="F35" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G35">
-        <v>405</v>
+        <v>535</v>
       </c>
       <c r="H35">
-        <v>3921</v>
+        <v>5095</v>
       </c>
       <c r="I35">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="J35">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>151</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
+      </c>
+      <c r="B36" t="s">
+        <v>144</v>
       </c>
       <c r="C36" t="s">
         <v>12</v>
       </c>
       <c r="D36">
-        <v>5.01</v>
+        <v>6.02</v>
       </c>
       <c r="E36" t="s">
-        <v>49</v>
+        <v>145</v>
       </c>
       <c r="F36" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G36">
-        <v>534</v>
+        <v>642</v>
       </c>
       <c r="H36">
-        <v>5293</v>
+        <v>7196</v>
       </c>
       <c r="I36">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="J36">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>154</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
+      </c>
+      <c r="B37" t="s">
+        <v>148</v>
       </c>
       <c r="C37" t="s">
         <v>12</v>
       </c>
       <c r="D37">
-        <v>4.43</v>
+        <v>3.8</v>
       </c>
       <c r="E37" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F37" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G37">
-        <v>472</v>
+        <v>405</v>
       </c>
       <c r="H37">
-        <v>4109</v>
+        <v>3921</v>
       </c>
       <c r="I37">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="J37">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>16</v>
+        <v>151</v>
+      </c>
+      <c r="B38" t="s">
+        <v>152</v>
       </c>
       <c r="C38" t="s">
         <v>12</v>
       </c>
       <c r="D38">
-        <v>4.0199999999999996</v>
+        <v>5.01</v>
       </c>
       <c r="E38" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="F38" t="s">
-        <v>18</v>
+        <v>153</v>
       </c>
       <c r="G38">
-        <v>428</v>
+        <v>534</v>
       </c>
       <c r="H38">
-        <v>3675</v>
+        <v>5293</v>
       </c>
       <c r="I38">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="J38">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>158</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>16</v>
+        <v>154</v>
+      </c>
+      <c r="B39" t="s">
+        <v>155</v>
       </c>
       <c r="C39" t="s">
         <v>12</v>
       </c>
       <c r="D39">
-        <v>4.0199999999999996</v>
+        <v>4.43</v>
       </c>
       <c r="E39" t="s">
-        <v>17</v>
+        <v>156</v>
       </c>
       <c r="F39" t="s">
-        <v>18</v>
+        <v>157</v>
       </c>
       <c r="G39">
-        <v>428</v>
+        <v>472</v>
       </c>
       <c r="H39">
-        <v>3675</v>
+        <v>4109</v>
       </c>
       <c r="I39">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="J39">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>159</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="B40" t="s">
+        <v>16</v>
       </c>
       <c r="C40" t="s">
         <v>12</v>
       </c>
       <c r="D40">
-        <v>4.05</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="E40" t="s">
-        <v>161</v>
+        <v>17</v>
       </c>
       <c r="F40" t="s">
-        <v>162</v>
+        <v>18</v>
       </c>
       <c r="G40">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H40">
-        <v>3791</v>
+        <v>3675</v>
       </c>
       <c r="I40">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J40">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>163</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
+      </c>
+      <c r="B41" t="s">
+        <v>160</v>
       </c>
       <c r="C41" t="s">
         <v>12</v>
       </c>
       <c r="D41">
-        <v>4.12</v>
+        <v>4.05</v>
       </c>
       <c r="E41" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F41" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G41">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="H41">
-        <v>4845</v>
+        <v>3791</v>
       </c>
       <c r="I41">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="J41">
-        <v>84</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>167</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
+      </c>
+      <c r="B42" t="s">
+        <v>164</v>
       </c>
       <c r="C42" t="s">
         <v>12</v>
       </c>
       <c r="D42">
-        <v>4</v>
+        <v>4.12</v>
       </c>
       <c r="E42" t="s">
-        <v>134</v>
+        <v>165</v>
       </c>
       <c r="F42" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="G42">
-        <v>426</v>
+        <v>439</v>
       </c>
       <c r="H42">
-        <v>3631</v>
+        <v>4845</v>
       </c>
       <c r="I42">
-        <v>135</v>
+        <v>153</v>
       </c>
       <c r="J42">
-        <v>110</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>170</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
+      </c>
+      <c r="B43" t="s">
+        <v>168</v>
       </c>
       <c r="C43" t="s">
         <v>12</v>
       </c>
       <c r="D43">
-        <v>4.01</v>
+        <v>4</v>
       </c>
       <c r="E43" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="F43" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G43">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H43">
-        <v>3889</v>
+        <v>3631</v>
       </c>
       <c r="I43">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="J43">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>174</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
+      </c>
+      <c r="B44" t="s">
+        <v>171</v>
       </c>
       <c r="C44" t="s">
         <v>12</v>
       </c>
       <c r="D44">
-        <v>10.050000000000001</v>
+        <v>4.01</v>
       </c>
       <c r="E44" t="s">
-        <v>93</v>
+        <v>172</v>
       </c>
       <c r="F44" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G44">
-        <v>1072</v>
+        <v>427</v>
       </c>
       <c r="H44">
-        <v>9304</v>
+        <v>3889</v>
       </c>
       <c r="I44">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J44">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>11</v>
+        <v>174</v>
+      </c>
+      <c r="B45" t="s">
+        <v>175</v>
       </c>
       <c r="C45" t="s">
         <v>12</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="E45" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="F45" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="G45">
-        <v>426</v>
+        <v>1072</v>
       </c>
       <c r="H45">
-        <v>3889</v>
+        <v>9304</v>
       </c>
       <c r="I45">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="J45">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>177</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
         <v>11</v>
       </c>
       <c r="C46" t="s">
@@ -2559,7 +2684,7 @@
       <c r="A47" t="s">
         <v>178</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" t="s">
         <v>179</v>
       </c>
       <c r="C47" t="s">
@@ -2591,7 +2716,7 @@
       <c r="A48" t="s">
         <v>182</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" t="s">
         <v>183</v>
       </c>
       <c r="C48" t="s">
@@ -2623,7 +2748,7 @@
       <c r="A49" t="s">
         <v>186</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" t="s">
         <v>187</v>
       </c>
       <c r="C49" t="s">
@@ -2655,7 +2780,7 @@
       <c r="A50" t="s">
         <v>190</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" t="s">
         <v>191</v>
       </c>
       <c r="C50" t="s">
@@ -2687,7 +2812,7 @@
       <c r="A51" t="s">
         <v>194</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" t="s">
         <v>195</v>
       </c>
       <c r="C51" t="s">
@@ -2719,7 +2844,7 @@
       <c r="A52" t="s">
         <v>198</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" t="s">
         <v>199</v>
       </c>
       <c r="C52" t="s">
@@ -2751,7 +2876,7 @@
       <c r="A53" t="s">
         <v>202</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" t="s">
         <v>203</v>
       </c>
       <c r="C53" t="s">
@@ -2783,7 +2908,7 @@
       <c r="A54" t="s">
         <v>206</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" t="s">
         <v>207</v>
       </c>
       <c r="C54" t="s">
@@ -2815,7 +2940,7 @@
       <c r="A55" t="s">
         <v>210</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" t="s">
         <v>211</v>
       </c>
       <c r="C55" t="s">
@@ -2847,7 +2972,7 @@
       <c r="A56" t="s">
         <v>214</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" t="s">
         <v>215</v>
       </c>
       <c r="C56" t="s">
@@ -2879,7 +3004,7 @@
       <c r="A57" t="s">
         <v>218</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" t="s">
         <v>219</v>
       </c>
       <c r="C57" t="s">
@@ -2911,7 +3036,7 @@
       <c r="A58" t="s">
         <v>222</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" t="s">
         <v>223</v>
       </c>
       <c r="C58" t="s">
@@ -2939,10 +3064,391 @@
         <v>116</v>
       </c>
     </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>226</v>
+      </c>
+      <c r="B59" t="s">
+        <v>227</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59">
+        <v>5.04</v>
+      </c>
+      <c r="E59" t="s">
+        <v>228</v>
+      </c>
+      <c r="F59" t="s">
+        <v>229</v>
+      </c>
+      <c r="G59">
+        <v>486</v>
+      </c>
+      <c r="H59">
+        <v>4246</v>
+      </c>
+      <c r="I59">
+        <v>144</v>
+      </c>
+      <c r="J59">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>230</v>
+      </c>
+      <c r="B60" t="s">
+        <v>231</v>
+      </c>
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60">
+        <v>3.04</v>
+      </c>
+      <c r="E60" t="s">
+        <v>232</v>
+      </c>
+      <c r="F60" t="s">
+        <v>233</v>
+      </c>
+      <c r="G60">
+        <v>293</v>
+      </c>
+      <c r="H60">
+        <v>2969</v>
+      </c>
+      <c r="I60">
+        <v>120</v>
+      </c>
+      <c r="J60">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>234</v>
+      </c>
+      <c r="B61" t="s">
+        <v>231</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61">
+        <v>3.04</v>
+      </c>
+      <c r="E61" t="s">
+        <v>232</v>
+      </c>
+      <c r="F61" t="s">
+        <v>233</v>
+      </c>
+      <c r="G61">
+        <v>293</v>
+      </c>
+      <c r="H61">
+        <v>2969</v>
+      </c>
+      <c r="I61">
+        <v>120</v>
+      </c>
+      <c r="J61">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>235</v>
+      </c>
+      <c r="B62" t="s">
+        <v>236</v>
+      </c>
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62">
+        <v>5.01</v>
+      </c>
+      <c r="E62" t="s">
+        <v>200</v>
+      </c>
+      <c r="F62" t="s">
+        <v>237</v>
+      </c>
+      <c r="G62">
+        <v>482</v>
+      </c>
+      <c r="H62">
+        <v>4639</v>
+      </c>
+      <c r="I62">
+        <v>144</v>
+      </c>
+      <c r="J62">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>238</v>
+      </c>
+      <c r="B63" t="s">
+        <v>239</v>
+      </c>
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>240</v>
+      </c>
+      <c r="F63" t="s">
+        <v>241</v>
+      </c>
+      <c r="G63">
+        <v>481</v>
+      </c>
+      <c r="H63">
+        <v>4449</v>
+      </c>
+      <c r="I63">
+        <v>147</v>
+      </c>
+      <c r="J63">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>242</v>
+      </c>
+      <c r="B64" t="s">
+        <v>243</v>
+      </c>
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>244</v>
+      </c>
+      <c r="F64" t="s">
+        <v>245</v>
+      </c>
+      <c r="G64">
+        <v>288</v>
+      </c>
+      <c r="H64">
+        <v>3128</v>
+      </c>
+      <c r="I64">
+        <v>142</v>
+      </c>
+      <c r="J64">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>246</v>
+      </c>
+      <c r="B65" t="s">
+        <v>247</v>
+      </c>
+      <c r="C65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65">
+        <v>5.27</v>
+      </c>
+      <c r="E65" t="s">
+        <v>248</v>
+      </c>
+      <c r="F65" t="s">
+        <v>249</v>
+      </c>
+      <c r="G65">
+        <v>508</v>
+      </c>
+      <c r="H65">
+        <v>4612</v>
+      </c>
+      <c r="I65">
+        <v>153</v>
+      </c>
+      <c r="J65">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>250</v>
+      </c>
+      <c r="B66" t="s">
+        <v>251</v>
+      </c>
+      <c r="C66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
+        <v>252</v>
+      </c>
+      <c r="F66" t="s">
+        <v>253</v>
+      </c>
+      <c r="G66">
+        <v>481</v>
+      </c>
+      <c r="H66">
+        <v>4889</v>
+      </c>
+      <c r="I66">
+        <v>144</v>
+      </c>
+      <c r="J66">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>254</v>
+      </c>
+      <c r="B67" t="s">
+        <v>255</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67">
+        <v>5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>256</v>
+      </c>
+      <c r="F67" t="s">
+        <v>257</v>
+      </c>
+      <c r="G67">
+        <v>481</v>
+      </c>
+      <c r="H67">
+        <v>4810</v>
+      </c>
+      <c r="I67">
+        <v>142</v>
+      </c>
+      <c r="J67">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>258</v>
+      </c>
+      <c r="B68" t="s">
+        <v>259</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68">
+        <v>4.24</v>
+      </c>
+      <c r="E68" t="s">
+        <v>260</v>
+      </c>
+      <c r="F68" t="s">
+        <v>261</v>
+      </c>
+      <c r="G68">
+        <v>409</v>
+      </c>
+      <c r="H68">
+        <v>3828</v>
+      </c>
+      <c r="I68">
+        <v>151</v>
+      </c>
+      <c r="J68">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>262</v>
+      </c>
+      <c r="B69" t="s">
+        <v>263</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69">
+        <v>4.03</v>
+      </c>
+      <c r="E69" t="s">
+        <v>120</v>
+      </c>
+      <c r="F69" t="s">
+        <v>264</v>
+      </c>
+      <c r="G69">
+        <v>388</v>
+      </c>
+      <c r="H69">
+        <v>4052</v>
+      </c>
+      <c r="I69">
+        <v>152</v>
+      </c>
+      <c r="J69">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>265</v>
+      </c>
+      <c r="B70" t="s">
+        <v>266</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70">
+        <v>10.01</v>
+      </c>
+      <c r="E70" t="s">
+        <v>267</v>
+      </c>
+      <c r="F70" t="s">
+        <v>268</v>
+      </c>
+      <c r="G70">
+        <v>964</v>
+      </c>
+      <c r="H70">
+        <v>10582</v>
+      </c>
+      <c r="I70">
+        <v>155</v>
+      </c>
+      <c r="J70">
+        <v>94</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J58">
-    <sortCondition ref="B2:B58"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>